<commit_message>
Actualizacion de Reporte de actividades
</commit_message>
<xml_diff>
--- a/Reporte Actividades/2023/1.Enero/16 ene.xlsx
+++ b/Reporte Actividades/2023/1.Enero/16 ene.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23265" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23268" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="FORMATO DE CONTROL DE ACTIVIDAD" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
   <si>
     <t xml:space="preserve">MA- MEJORAS Y MANTENIMIENTO DE APLICACIONES </t>
   </si>
@@ -195,9 +195,6 @@
     <t>Enrutamiento de entradas y salidas y variables del VSD en aplicación Monopozo AFE</t>
   </si>
   <si>
-    <t>Soporte caño sur entradas analogas no funcionales, validacion de aplicación, y cambio de ip para segmento de posicion del cluster</t>
-  </si>
-  <si>
     <t>Alistamiento de VSD para pruebas de comunicación Apiay equipo de 500</t>
   </si>
   <si>
@@ -214,6 +211,27 @@
   </si>
   <si>
     <t>Configuracion de pantallas para skids</t>
+  </si>
+  <si>
+    <t>Liberacion y configuracion de Equipo 300 KVA Update Ecopetrol</t>
+  </si>
+  <si>
+    <t>NLB</t>
+  </si>
+  <si>
+    <t>Soporte Rubiales Entradas Analogas equipo de 300 KVA, soporte Bull USA Toma de referencia desde libreria nodePCCC</t>
+  </si>
+  <si>
+    <t>Liberacion de Equipo 300 Upgrade Ecopetrol</t>
+  </si>
+  <si>
+    <t>Soporte caño sur entradas analogas no funcionales, validacion de aplicación, y cambio de ip para segmento de posicion del cluster Sergio Mejia</t>
+  </si>
+  <si>
+    <t>Ajuste de comunicacion Equipo de Frontera 300 kva adicion de disparo de tension logica actualizada, disparo despues de 5 seg</t>
+  </si>
+  <si>
+    <t>Cambio de Estructura de IO dinamicas y entradas y salidas de PLC aplicacion Monopozo  AFE</t>
   </si>
 </sst>
 </file>
@@ -470,10 +488,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,28 +506,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -544,32 +574,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1749,7 +1767,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2081,147 +2099,147 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11:N12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9:T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="3" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="33.28515625" customWidth="1"/>
-    <col min="15" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="33.33203125" customWidth="1"/>
+    <col min="15" max="16" width="11.44140625" customWidth="1"/>
+    <col min="17" max="17" width="8.5546875" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" customWidth="1"/>
     <col min="19" max="19" width="6" customWidth="1"/>
-    <col min="20" max="20" width="6.28515625" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" customWidth="1"/>
+    <col min="20" max="20" width="6.33203125" customWidth="1"/>
+    <col min="21" max="21" width="8.5546875" customWidth="1"/>
     <col min="22" max="22" width="20" customWidth="1"/>
     <col min="23" max="23" width="6" customWidth="1"/>
-    <col min="24" max="24" width="6.5703125" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" customWidth="1"/>
-    <col min="26" max="26" width="12.5703125" customWidth="1"/>
+    <col min="24" max="24" width="6.5546875" customWidth="1"/>
+    <col min="25" max="25" width="9.6640625" customWidth="1"/>
+    <col min="26" max="26" width="12.5546875" customWidth="1"/>
     <col min="27" max="27" width="7" customWidth="1"/>
-    <col min="28" max="28" width="6.5703125" customWidth="1"/>
+    <col min="28" max="28" width="6.5546875" customWidth="1"/>
     <col min="29" max="29" width="10" customWidth="1"/>
-    <col min="30" max="30" width="26.5703125" customWidth="1"/>
+    <col min="30" max="30" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="23.25" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="13" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="38" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:30">
-      <c r="A2" s="16"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="13"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="38"/>
     </row>
     <row r="3" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="9" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9" t="s">
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="14" t="s">
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="39" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2229,35 +2247,35 @@
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="14"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="39"/>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1">
       <c r="A5" s="6" t="s">
@@ -2426,472 +2444,512 @@
       <c r="AD6" s="5"/>
     </row>
     <row r="7" spans="1:30" ht="18" customHeight="1">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="12" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="9">
         <v>50</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="39">
+      <c r="O7" s="14">
         <v>80</v>
       </c>
-      <c r="P7" s="39" t="s">
+      <c r="P7" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="39" t="s">
+      <c r="Q7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="8"/>
+      <c r="R7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="S7" s="9">
+        <v>50</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
     </row>
-    <row r="8" spans="1:30" ht="82.9" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
+    <row r="8" spans="1:30" ht="82.95" customHeight="1">
+      <c r="A8" s="25"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
     </row>
     <row r="9" spans="1:30" ht="72.75" customHeight="1">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="9">
         <v>50</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
     </row>
     <row r="10" spans="1:30" ht="105.75" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
     </row>
     <row r="11" spans="1:30" ht="96" customHeight="1">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="9">
         <v>50</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="9">
+        <v>50</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="36"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="S11" s="9">
+        <v>50</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="V11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="W11" s="9">
+        <v>40</v>
+      </c>
+      <c r="X11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z11" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="8">
+      <c r="AA11" s="9">
+        <v>80</v>
+      </c>
+      <c r="AB11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="AC11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD11" s="9"/>
+    </row>
+    <row r="12" spans="1:30" ht="103.95" customHeight="1">
+      <c r="A12" s="25"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+    </row>
+    <row r="13" spans="1:30" ht="58.95" customHeight="1">
+      <c r="A13" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="9">
         <v>50</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="H13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="8"/>
+      <c r="J13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="9">
+        <v>30</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" s="14">
+        <v>20</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="R13" s="10"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W13" s="12">
+        <v>60</v>
+      </c>
+      <c r="X13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
     </row>
-    <row r="12" spans="1:30" ht="103.9" customHeight="1">
-      <c r="A12" s="21"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="8"/>
-    </row>
-    <row r="13" spans="1:30" ht="58.9" customHeight="1">
-      <c r="A13" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="8">
-        <v>50</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K13" s="8">
-        <v>30</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="N13" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="O13" s="39">
-        <v>20</v>
-      </c>
-      <c r="P13" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q13" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="R13" s="18"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="10"/>
-      <c r="AA13" s="10"/>
-      <c r="AB13" s="10"/>
-      <c r="AC13" s="10"/>
-      <c r="AD13" s="10"/>
-    </row>
-    <row r="14" spans="1:30" ht="143.44999999999999" customHeight="1">
-      <c r="A14" s="23"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
+    <row r="14" spans="1:30" ht="143.4" customHeight="1">
+      <c r="A14" s="27"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
       <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="13"/>
     </row>
     <row r="15" spans="1:30">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
     </row>
     <row r="16" spans="1:30">
-      <c r="A16" s="17"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
     </row>
-    <row r="17" spans="1:50" ht="19.149999999999999" customHeight="1">
-      <c r="A17" s="36" t="s">
+    <row r="17" spans="1:50" ht="19.2" customHeight="1">
+      <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17" s="8">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="9">
         <v>20</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="N17" s="12"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
     </row>
     <row r="18" spans="1:50" ht="91.5" customHeight="1">
-      <c r="A18" s="37"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="8"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
     </row>
     <row r="19" spans="1:50">
       <c r="A19" s="1"/>
@@ -2998,10 +3056,10 @@
       <c r="AX20" s="1"/>
     </row>
     <row r="21" spans="1:50">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -3052,10 +3110,10 @@
       <c r="AX21" s="1"/>
     </row>
     <row r="22" spans="1:50">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -3106,10 +3164,10 @@
       <c r="AX22" s="1"/>
     </row>
     <row r="23" spans="1:50">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -3629,6 +3687,172 @@
     </row>
   </sheetData>
   <mergeCells count="190">
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="L3:U4"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AA15:AA16"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="B1:AC2"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AC11:AC12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="AD17:AD18"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="V3:AC4"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B3:K4"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="H13:H14"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="P17:P18"/>
@@ -3653,172 +3877,6 @@
     <mergeCell ref="Q9:Q10"/>
     <mergeCell ref="N17:N18"/>
     <mergeCell ref="O13:O14"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Y15:Y16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AD11:AD12"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B3:K4"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="B1:AC2"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AC11:AC12"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="AD17:AD18"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V3:AC4"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="L3:U4"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="Z7:Z8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>